<commit_message>
Updated BSD - Protocol
</commit_message>
<xml_diff>
--- a/BSD - Protokoll.xlsx
+++ b/BSD - Protokoll.xlsx
@@ -119,10 +119,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,27 +542,27 @@
       <c r="B2" s="3"/>
     </row>
     <row r="5" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="W5" s="4" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="W5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -624,7 +624,7 @@
       <c r="F7" s="1">
         <v>0.61111111111111105</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="M7" t="s">
@@ -639,7 +639,7 @@
       <c r="P7" s="1">
         <v>0.61111111111111105</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="W7" t="s">
@@ -654,7 +654,7 @@
       <c r="Z7" s="1">
         <v>0.61111111111111105</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AA7" s="4">
         <v>1</v>
       </c>
     </row>
@@ -669,9 +669,9 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="F8" s="1">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="G8" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="G8" s="4">
         <v>0.7</v>
       </c>
       <c r="M8" t="s">
@@ -684,9 +684,9 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="P8" s="1">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="Q8" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="Q8" s="4">
         <v>1</v>
       </c>
       <c r="W8" t="s">
@@ -699,9 +699,9 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="Z8" s="1">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="AA8" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="AA8" s="4">
         <v>0.7</v>
       </c>
     </row>
@@ -709,449 +709,449 @@
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="N9" s="2"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="4"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="5"/>
+      <c r="AA9" s="4"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="N10" s="2"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="4"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="5"/>
+      <c r="AA10" s="4"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="5"/>
+      <c r="Q11" s="4"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="5"/>
+      <c r="AA11" s="4"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="4"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="5"/>
+      <c r="AA12" s="4"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="4"/>
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="5"/>
+      <c r="Q13" s="4"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="5"/>
+      <c r="AA13" s="4"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="N14" s="2"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="4"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
-      <c r="AA14" s="5"/>
+      <c r="AA14" s="4"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="N15" s="2"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="5"/>
+      <c r="Q15" s="4"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="5"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
       <c r="N16" s="2"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="5"/>
+      <c r="Q16" s="4"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="5"/>
+      <c r="AA16" s="4"/>
     </row>
     <row r="17" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="N17" s="2"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="4"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="5"/>
+      <c r="AA17" s="4"/>
     </row>
     <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="5"/>
+      <c r="G18" s="4"/>
       <c r="N18" s="2"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="5"/>
+      <c r="Q18" s="4"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="5"/>
+      <c r="AA18" s="4"/>
     </row>
     <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="N19" s="2"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="5"/>
+      <c r="Q19" s="4"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="5"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
       <c r="N20" s="2"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="5"/>
+      <c r="Q20" s="4"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="5"/>
+      <c r="AA20" s="4"/>
     </row>
     <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
       <c r="N21" s="2"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="5"/>
+      <c r="Q21" s="4"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="5"/>
+      <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="5"/>
+      <c r="G22" s="4"/>
       <c r="N22" s="2"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="5"/>
+      <c r="Q22" s="4"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="5"/>
+      <c r="AA22" s="4"/>
     </row>
     <row r="23" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="4"/>
       <c r="N23" s="2"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="5"/>
+      <c r="Q23" s="4"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="5"/>
+      <c r="AA23" s="4"/>
     </row>
     <row r="24" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="4"/>
       <c r="N24" s="2"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="5"/>
+      <c r="Q24" s="4"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="5"/>
+      <c r="AA24" s="4"/>
     </row>
     <row r="25" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="5"/>
+      <c r="G25" s="4"/>
       <c r="N25" s="2"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="5"/>
+      <c r="Q25" s="4"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="5"/>
+      <c r="AA25" s="4"/>
     </row>
     <row r="26" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="4"/>
       <c r="N26" s="2"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="5"/>
+      <c r="Q26" s="4"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
-      <c r="AA26" s="5"/>
+      <c r="AA26" s="4"/>
     </row>
     <row r="27" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="4"/>
       <c r="N27" s="2"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="5"/>
+      <c r="Q27" s="4"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="5"/>
+      <c r="AA27" s="4"/>
     </row>
     <row r="28" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="4"/>
       <c r="N28" s="2"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="5"/>
+      <c r="Q28" s="4"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="5"/>
+      <c r="AA28" s="4"/>
     </row>
     <row r="29" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="4"/>
       <c r="N29" s="2"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="5"/>
+      <c r="Q29" s="4"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="5"/>
+      <c r="AA29" s="4"/>
     </row>
     <row r="30" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="4"/>
       <c r="N30" s="2"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="5"/>
+      <c r="Q30" s="4"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
-      <c r="AA30" s="5"/>
+      <c r="AA30" s="4"/>
     </row>
     <row r="31" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="5"/>
+      <c r="G31" s="4"/>
       <c r="N31" s="2"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="5"/>
+      <c r="Q31" s="4"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="5"/>
+      <c r="AA31" s="4"/>
     </row>
     <row r="32" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="4"/>
       <c r="N32" s="2"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-      <c r="Q32" s="5"/>
+      <c r="Q32" s="4"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
-      <c r="AA32" s="5"/>
+      <c r="AA32" s="4"/>
     </row>
     <row r="33" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="4"/>
       <c r="N33" s="2"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="5"/>
+      <c r="Q33" s="4"/>
       <c r="X33" s="2"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="5"/>
+      <c r="AA33" s="4"/>
     </row>
     <row r="34" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="5"/>
+      <c r="G34" s="4"/>
       <c r="N34" s="2"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="5"/>
+      <c r="Q34" s="4"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
-      <c r="AA34" s="5"/>
+      <c r="AA34" s="4"/>
     </row>
     <row r="35" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="4"/>
       <c r="N35" s="2"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="5"/>
+      <c r="Q35" s="4"/>
       <c r="X35" s="2"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
-      <c r="AA35" s="5"/>
+      <c r="AA35" s="4"/>
     </row>
     <row r="36" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="5"/>
+      <c r="G36" s="4"/>
       <c r="N36" s="2"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="5"/>
+      <c r="Q36" s="4"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
-      <c r="AA36" s="5"/>
+      <c r="AA36" s="4"/>
     </row>
     <row r="37" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="4"/>
       <c r="N37" s="2"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-      <c r="Q37" s="5"/>
+      <c r="Q37" s="4"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
-      <c r="AA37" s="5"/>
+      <c r="AA37" s="4"/>
     </row>
     <row r="38" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="4"/>
       <c r="N38" s="2"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
-      <c r="Q38" s="5"/>
+      <c r="Q38" s="4"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
-      <c r="AA38" s="5"/>
+      <c r="AA38" s="4"/>
     </row>
     <row r="39" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="4"/>
       <c r="N39" s="2"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
-      <c r="Q39" s="5"/>
+      <c r="Q39" s="4"/>
       <c r="X39" s="2"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
-      <c r="AA39" s="5"/>
+      <c r="AA39" s="4"/>
     </row>
     <row r="40" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="5"/>
+      <c r="G40" s="4"/>
       <c r="N40" s="2"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="5"/>
+      <c r="Q40" s="4"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
-      <c r="AA40" s="5"/>
+      <c r="AA40" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updated BSD - Arbeitsprotokoll
</commit_message>
<xml_diff>
--- a/BSD - Protokoll.xlsx
+++ b/BSD - Protokoll.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Lamprecht Daniel</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Protokollerstellung</t>
+  </si>
+  <si>
+    <t>Erstellung des Logischen Modells</t>
+  </si>
+  <si>
+    <t>Erstellung der Create Tables</t>
   </si>
 </sst>
 </file>
@@ -510,30 +516,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.75" customWidth="1"/>
+    <col min="12" max="12" width="5.75" customWidth="1"/>
+    <col min="13" max="13" width="43.75" customWidth="1"/>
+    <col min="14" max="14" width="17.125" customWidth="1"/>
+    <col min="15" max="15" width="16.625" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="36.5703125" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.875" customWidth="1"/>
+    <col min="23" max="23" width="36.625" customWidth="1"/>
+    <col min="24" max="24" width="20.375" customWidth="1"/>
+    <col min="25" max="25" width="13.25" customWidth="1"/>
+    <col min="26" max="26" width="17.25" customWidth="1"/>
     <col min="27" max="27" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -672,7 +678,7 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="G8" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="M8" t="s">
         <v>10</v>
@@ -702,7 +708,7 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="AA8" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -710,10 +716,21 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="4"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="4"/>
+      <c r="M9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="2">
+        <v>42647</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>1</v>
+      </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -724,10 +741,21 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="4"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="4"/>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="2">
+        <v>42647</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1</v>
+      </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>

</xml_diff>